<commit_message>
Registro de configuración de factores 80%, registro y actualización. Falta.
</commit_message>
<xml_diff>
--- a/back-end/Web-CH-G-v2/INDICADORES_DINAMICOS.xlsx
+++ b/back-end/Web-CH-G-v2/INDICADORES_DINAMICOS.xlsx
@@ -2,19 +2,19 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eduardo\MRVMinem\Web-CH-G-v2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DGEE\mrv-minem\back-end\Web-CH-G-v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17265"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17270"/>
   </bookViews>
   <sheets>
     <sheet name="INDICADORES-FACTORES" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -479,7 +479,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,6 +648,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -666,7 +667,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Entrada" xfId="1" builtinId="20"/>
@@ -1284,52 +1284,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="F95" sqref="F95"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.42578125" customWidth="1"/>
+    <col min="1" max="1" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" customWidth="1"/>
+    <col min="3" max="3" width="18.453125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.26953125" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="29.453125" customWidth="1"/>
     <col min="13" max="13" width="24" customWidth="1"/>
     <col min="14" max="14" width="17" customWidth="1"/>
     <col min="15" max="15" width="30" customWidth="1"/>
-    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16"/>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="15"/>
-      <c r="J3" s="18" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="A3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="16"/>
+      <c r="J3" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="K3" s="18"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="K3" s="19"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -1382,7 +1382,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1431,7 +1431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -1533,7 +1533,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>4</v>
       </c>
@@ -1586,7 +1586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -1639,7 +1639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -1688,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -1741,7 +1741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>8</v>
       </c>
@@ -1794,7 +1794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>9</v>
       </c>
@@ -1847,7 +1847,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>10</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>11</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="J16" s="2">
         <v>9</v>
       </c>
@@ -1982,17 +1982,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
         <v>146</v>
       </c>
-      <c r="B19" s="17"/>
-      <c r="J19" s="18" t="s">
+      <c r="B19" s="18"/>
+      <c r="J19" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="K19" s="18"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K19" s="19"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>2</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>1</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>1</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>1</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>1</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>1</v>
       </c>
@@ -2143,7 +2143,7 @@
       <c r="L25" s="2"/>
       <c r="M25" s="2"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>1</v>
       </c>
@@ -2161,7 +2161,7 @@
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>3</v>
       </c>
@@ -2179,7 +2179,7 @@
       <c r="L27" s="2"/>
       <c r="M27" s="2"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>3</v>
       </c>
@@ -2197,7 +2197,7 @@
       <c r="L28" s="2"/>
       <c r="M28" s="2"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>3</v>
       </c>
@@ -2211,7 +2211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>3</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>6</v>
       </c>
@@ -2239,7 +2239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>6</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>6</v>
       </c>
@@ -2267,7 +2267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>6</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>6</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>6</v>
       </c>
@@ -2309,17 +2309,17 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A42" s="18" t="s">
         <v>147</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="J42" s="17" t="s">
+      <c r="B42" s="18"/>
+      <c r="J42" s="18" t="s">
         <v>148</v>
       </c>
-      <c r="K42" s="17"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K42" s="18"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>31</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>3</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>3</v>
       </c>
@@ -2442,7 +2442,7 @@
         <v>42755</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>3</v>
       </c>
@@ -2483,7 +2483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>3</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>3</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>3</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>3</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>3</v>
       </c>
@@ -2688,7 +2688,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" s="2"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2715,7 +2715,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J53" s="2">
         <v>1</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>42755</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J54" s="2">
         <v>1</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J55" s="2">
         <v>1</v>
       </c>
@@ -2775,7 +2775,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="J56" s="2">
         <v>1</v>
       </c>
@@ -2795,11 +2795,11 @@
         <v>4800</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" s="15" t="s">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A57" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="B57" s="15"/>
+      <c r="B57" s="16"/>
       <c r="J57" s="2">
         <v>1</v>
       </c>
@@ -2819,7 +2819,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" s="4" t="s">
         <v>110</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>1</v>
       </c>
@@ -2871,7 +2871,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>2</v>
       </c>
@@ -2879,7 +2879,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>3</v>
       </c>
@@ -2887,7 +2887,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>4</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>5</v>
       </c>
@@ -2903,7 +2903,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>6</v>
       </c>
@@ -2911,18 +2911,18 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:15" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
+    <row r="67" spans="1:15" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="B67" s="19"/>
-      <c r="C67" s="19"/>
-      <c r="K67" s="20" t="s">
+      <c r="B67" s="20"/>
+      <c r="C67" s="20"/>
+      <c r="K67" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="L67" s="20"/>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L67" s="21"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A68" s="4" t="s">
         <v>110</v>
       </c>
@@ -2966,7 +2966,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>1</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>187.35810000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>1</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>187.35810000000001</v>
       </c>
     </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>1</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>187.35810000000001</v>
       </c>
     </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>1</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>11.346</v>
       </c>
     </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>2</v>
       </c>
@@ -3168,7 +3168,7 @@
         <v>11.346</v>
       </c>
     </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>2</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>11.346</v>
       </c>
     </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>3</v>
       </c>
@@ -3250,7 +3250,7 @@
         <v>0.108</v>
       </c>
     </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>3</v>
       </c>
@@ -3292,7 +3292,7 @@
         <v>189.2458</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>4</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>189.2458</v>
       </c>
     </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>4</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>189.2458</v>
       </c>
     </row>
-    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>5</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>5</v>
       </c>
@@ -3424,7 +3424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>5</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>5</v>
       </c>
@@ -3476,13 +3476,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="15" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A90" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="B90" s="15"/>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B90" s="16"/>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="4" t="s">
         <v>2</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>9</v>
       </c>
@@ -3532,7 +3532,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>10</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>11</v>
       </c>
@@ -3580,8 +3580,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="D95" s="21" t="s">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="D95" s="15" t="s">
         <v>133</v>
       </c>
       <c r="E95">
@@ -3589,12 +3589,12 @@
       </c>
       <c r="F95" s="2"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="13" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A97" s="14" t="s">
         <v>128</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A98" s="14" t="s">
         <v>132</v>
       </c>
@@ -3610,7 +3610,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A99" s="14" t="s">
         <v>133</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A110">
         <f>(57600*20*187.3581)/1000000</f>
         <v>215.83653120000002</v>

</xml_diff>